<commit_message>
Lab 01: prezenta semigrupa 1.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>Nr.</t>
   </si>
@@ -187,13 +187,16 @@
     <t>P</t>
   </si>
   <si>
-    <t>Vranau V. Flavius Silviu (gr 4)</t>
-  </si>
-  <si>
-    <t>Dulau I. Marius Cristian (joi gr 4 sem 1)</t>
-  </si>
-  <si>
-    <t>Prata L. Dragos Liviu (gr 4)</t>
+    <t>Prata L. Dragos Liviu (mutat gr 4)</t>
+  </si>
+  <si>
+    <t>Vranau V. Flavius Silviu (mutat gr 4)</t>
+  </si>
+  <si>
+    <t>Bompa Flaviu (venit din gr 4)</t>
+  </si>
+  <si>
+    <t>Dulau I. Marius Cristian (mutat gr 4)</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
   <dimension ref="A1:AA39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -925,7 +928,9 @@
       <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -940,8 +945,8 @@
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
       <c r="Q3" s="17">
-        <f t="shared" ref="Q2:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
-        <v>0</v>
+        <f t="shared" ref="Q3:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="R3" s="21"/>
       <c r="S3" s="10"/>
@@ -999,7 +1004,9 @@
       <c r="B5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
@@ -1015,7 +1022,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="21"/>
       <c r="S5" s="10"/>
@@ -1034,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>54</v>
@@ -1075,7 +1082,9 @@
       <c r="B7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
@@ -1091,7 +1100,7 @@
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="10"/>
@@ -1112,7 +1121,9 @@
       <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
@@ -1128,7 +1139,7 @@
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="17"/>
       <c r="S8" s="10"/>
@@ -1149,7 +1160,9 @@
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="26"/>
+      <c r="C9" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
@@ -1165,7 +1178,7 @@
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="10"/>
@@ -1186,7 +1199,9 @@
       <c r="B10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
@@ -1202,7 +1217,7 @@
       <c r="P10" s="17"/>
       <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="10"/>
@@ -1223,7 +1238,9 @@
       <c r="B11" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -1239,7 +1256,7 @@
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="10"/>
@@ -1260,7 +1277,9 @@
       <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D12" s="17"/>
       <c r="E12" s="27"/>
       <c r="F12" s="17"/>
@@ -1276,7 +1295,7 @@
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12" s="17"/>
       <c r="S12" s="10"/>
@@ -1297,7 +1316,9 @@
       <c r="B13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
@@ -1313,7 +1334,7 @@
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="10"/>
@@ -1373,7 +1394,9 @@
       <c r="B15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
@@ -1389,7 +1412,7 @@
       <c r="P15" s="21"/>
       <c r="Q15" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="10"/>
@@ -1486,7 +1509,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>54</v>
@@ -1718,7 +1741,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>54</v>
@@ -1789,9 +1812,15 @@
       <c r="AA25" s="10"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="14"/>
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>

</xml_diff>